<commit_message>
Add task of 2nd Nov
</commit_message>
<xml_diff>
--- a/2nd_semester_syllabus.xlsx
+++ b/2nd_semester_syllabus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UBIT-Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC9FF2-F922-47CA-98D4-F2F2930C1934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818A904B-9D05-4401-A732-48BF6D7A1BFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{FE5F6B1B-E505-499C-8EC6-799EE1C40C02}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>Code</t>
   </si>
@@ -250,10 +250,19 @@
     <t>complete Assignment of LA</t>
   </si>
   <si>
-    <t>Write Summary of Chap 1, 2 BCS</t>
-  </si>
-  <si>
     <t>Complete Calculus 12.1 Assignments</t>
+  </si>
+  <si>
+    <t>Write Summary of Chap 1 (half)</t>
+  </si>
+  <si>
+    <t>Complete Calculus 12.2 Assignments</t>
+  </si>
+  <si>
+    <t>Write Summary of Chap 1 (other half)</t>
+  </si>
+  <si>
+    <t>Complete Calculus 14.1 Assignment</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AC2529-B6A2-4150-831B-47AB7EAC019E}">
-  <dimension ref="A3:B24"/>
+  <dimension ref="A3:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,124 +1122,137 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A5">
         <f>A3+1</f>
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ref="A7:A24" si="0">A6+1</f>
-        <v>3</v>
+      <c r="B7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="B8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>A5+1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" ref="A10:A26" si="0">A9+1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>

</xml_diff>